<commit_message>
Changing point size, grouping cortisol results
</commit_message>
<xml_diff>
--- a/output/CortisolELISAvalues.xlsx
+++ b/output/CortisolELISAvalues.xlsx
@@ -35,9 +35,6 @@
     <t>OD_570</t>
   </si>
   <si>
-    <t>PB_24</t>
-  </si>
-  <si>
     <t>viability_1hr</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>dilutionCorrected_conc</t>
+  </si>
+  <si>
+    <t>Ro_conc</t>
   </si>
   <si>
     <t>1</t>

</xml_diff>